<commit_message>
pulled in new raw data for clustering and worked on Kanae's data
</commit_message>
<xml_diff>
--- a/case_study_analysis/make_clean_data/raw/Yuga and Gaku SNAPP Case Study_.xlsx
+++ b/case_study_analysis/make_clean_data/raw/Yuga and Gaku SNAPP Case Study_.xlsx
@@ -7169,7 +7169,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7197,7 +7197,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>

<commit_message>
Updated raw data and changed spelling for Galicia case study
</commit_message>
<xml_diff>
--- a/case_study_analysis/make_clean_data/raw/Yuga and Gaku SNAPP Case Study_.xlsx
+++ b/case_study_analysis/make_clean_data/raw/Yuga and Gaku SNAPP Case Study_.xlsx
@@ -7141,7 +7141,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7169,7 +7169,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -7197,7 +7197,7 @@
     <xdr:ext cx="3105150" cy="2152650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="画像"/>
+        <xdr:cNvPr id="0" name="image3.png" title="画像"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>

</xml_diff>